<commit_message>
start converting to wc_lang model representation build private_species() and find_shared_species()
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model_for_access_species_populations.xlsx
+++ b/tests/fixtures/test_model_for_access_species_populations.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1460" windowWidth="25600" windowHeight="15540" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -422,7 +422,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -440,7 +440,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -952,10 +951,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -991,9 +990,6 @@
       <c r="J1" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1065,10 +1061,10 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="202" zoomScaleNormal="202" zoomScalePageLayoutView="202" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A18"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1148,7 +1144,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1226,10 +1222,10 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1490,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>